<commit_message>
Done with adding effort level field
</commit_message>
<xml_diff>
--- a/enhancements.xlsx
+++ b/enhancements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Form</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Remove Back link</t>
+  </si>
+  <si>
+    <t>Done - can't repropuce error</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,6 +657,9 @@
       <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="C12" t="s">
@@ -662,6 +668,9 @@
       <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
@@ -683,6 +692,9 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="1" customFormat="1">

</xml_diff>

<commit_message>
Done with loading multiple but really single file upload
</commit_message>
<xml_diff>
--- a/enhancements.xlsx
+++ b/enhancements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Form</t>
   </si>
@@ -123,9 +123,6 @@
     <t>users should be able to upload pictures</t>
   </si>
   <si>
-    <t>users should be able to email a recipe</t>
-  </si>
-  <si>
     <t>Link other recipes</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Done - can't repropuce error</t>
+  </si>
+  <si>
+    <t>capability to email the recipe</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,7 +658,7 @@
         <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -685,51 +685,54 @@
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="D16" t="s">
+    <row r="17" spans="3:4">
+      <c r="D17" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="D17" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="30">
       <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>